<commit_message>
hmmcore run on 1208 finished
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/species_list_10071623_NJMg.xlsx
+++ b/flag/AQB_classification/species_list_10071623_NJMg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/Downloads/iqtree_genomes_wLitLinks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A55D13A-5FB2-0547-8E91-4EFA4E52A7E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF2587C-3426-3341-A784-727BCA17EC4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="500" windowWidth="35160" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="600" windowWidth="35160" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_list_10071623_NJMf" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5368" uniqueCount="2926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5384" uniqueCount="2932">
   <si>
     <t>Download script?</t>
   </si>
@@ -8791,13 +8791,32 @@
     <t>Escherichia coli 042 1_2</t>
   </si>
   <si>
-    <t>PRJEB3868_Verrucomicrobium_sp</t>
-  </si>
-  <si>
-    <t>PRJEB38681_Verrucomicrobium_sp</t>
-  </si>
-  <si>
     <t>downloaded 2023-07-26</t>
+  </si>
+  <si>
+    <t>ASM2712v1</t>
+  </si>
+  <si>
+    <t>GCA_000027125.1</t>
+  </si>
+  <si>
+    <t>GCF_000027125.1</t>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>formerly PRJEB3868_Verrucomicrobium_sp</t>
+  </si>
+  <si>
+    <t>formerly 
+PRJEB38681_Verrucomicrobium_sp</t>
+  </si>
+  <si>
+    <t>VER_PRJEB3868.0_CAIZXV01</t>
+  </si>
+  <si>
+    <t>VER_PRJEB38681.0_CAISZB01</t>
   </si>
 </sst>
 </file>
@@ -9281,10 +9300,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9640,13 +9663,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH392"/>
+  <dimension ref="A1:AH393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="15" ySplit="1" topLeftCell="P356" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="15" ySplit="1" topLeftCell="AB198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O391" sqref="O391"/>
+      <selection pane="bottomRight" activeCell="C228" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18128,9 +18151,12 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="227" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B227" s="4" t="s">
+        <v>2928</v>
+      </c>
       <c r="C227" t="s">
-        <v>2923</v>
+        <v>2930</v>
       </c>
       <c r="D227" t="s">
         <v>1660</v>
@@ -18169,9 +18195,12 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="228" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B228" s="4" t="s">
+        <v>2929</v>
+      </c>
       <c r="C228" t="s">
-        <v>2924</v>
+        <v>2931</v>
       </c>
       <c r="D228" t="s">
         <v>1661</v>
@@ -26316,7 +26345,7 @@
     </row>
     <row r="381" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="B381" t="s">
         <v>2532</v>
@@ -26666,7 +26695,7 @@
     </row>
     <row r="388" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C388" t="s">
         <v>2871</v>
@@ -26807,7 +26836,7 @@
     </row>
     <row r="391" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C391" t="s">
         <v>2897</v>
@@ -26896,7 +26925,54 @@
         <v>1837</v>
       </c>
     </row>
+    <row r="393" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C393" t="s">
+        <v>2925</v>
+      </c>
+      <c r="D393" t="s">
+        <v>2926</v>
+      </c>
+      <c r="F393" t="s">
+        <v>2924</v>
+      </c>
+      <c r="H393" t="s">
+        <v>39</v>
+      </c>
+      <c r="I393" t="s">
+        <v>51</v>
+      </c>
+      <c r="J393" t="s">
+        <v>52</v>
+      </c>
+      <c r="K393" t="s">
+        <v>238</v>
+      </c>
+      <c r="L393" t="s">
+        <v>715</v>
+      </c>
+      <c r="M393" t="s">
+        <v>716</v>
+      </c>
+      <c r="N393" t="s">
+        <v>717</v>
+      </c>
+      <c r="O393" s="3" t="s">
+        <v>2927</v>
+      </c>
+      <c r="AE393" t="s">
+        <v>2922</v>
+      </c>
+      <c r="AG393" t="s">
+        <v>2281</v>
+      </c>
+      <c r="AH393" t="s">
+        <v>1837</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="O393" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
linked up to new tipnames on hmmcore
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/species_list_10071623_NJMg.xlsx
+++ b/flag/AQB_classification/species_list_10071623_NJMg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/Downloads/iqtree_genomes_wLitLinks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/bioinfRhints/flag/AQB_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE0BA15-D04F-4E4F-9E3C-4CC5BA1BE8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D22A9D-6E9C-5047-8925-6D65D7D4D811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="5320" windowWidth="35160" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9789,7 +9789,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9803,10 +9803,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10166,15 +10163,14 @@
   <dimension ref="A1:AY439"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="15" ySplit="1" topLeftCell="P378" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="15" ySplit="1" topLeftCell="Z378" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B417" sqref="B417"/>
+      <selection pane="bottomRight" activeCell="K391" sqref="K391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="17" width="10.83203125" style="12"/>
     <col min="31" max="31" width="40.6640625" customWidth="1"/>
     <col min="33" max="33" width="15" customWidth="1"/>
   </cols>
@@ -10222,10 +10218,10 @@
       <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="R1" s="2" t="s">
@@ -10358,7 +10354,7 @@
       <c r="O3" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -10548,10 +10544,10 @@
       <c r="O8" t="s">
         <v>112</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" t="s">
         <v>113</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" t="s">
         <v>114</v>
       </c>
     </row>
@@ -10595,7 +10591,7 @@
       <c r="O9" t="s">
         <v>116</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="P9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -10674,7 +10670,7 @@
       <c r="O11">
         <v>168</v>
       </c>
-      <c r="Q11" s="12" t="s">
+      <c r="Q11" t="s">
         <v>139</v>
       </c>
     </row>
@@ -10750,7 +10746,7 @@
       <c r="O13" t="s">
         <v>161</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P13" t="s">
         <v>162</v>
       </c>
     </row>
@@ -10890,7 +10886,7 @@
       <c r="O17" t="s">
         <v>191</v>
       </c>
-      <c r="P17" s="12" t="s">
+      <c r="P17" t="s">
         <v>192</v>
       </c>
     </row>
@@ -10934,7 +10930,7 @@
       <c r="O18" t="s">
         <v>203</v>
       </c>
-      <c r="Q18" s="12" t="s">
+      <c r="Q18" t="s">
         <v>204</v>
       </c>
     </row>
@@ -10972,7 +10968,7 @@
       <c r="O19" t="s">
         <v>212</v>
       </c>
-      <c r="Q19" s="12" t="s">
+      <c r="Q19" t="s">
         <v>139</v>
       </c>
     </row>
@@ -11320,7 +11316,7 @@
       <c r="O28" t="s">
         <v>273</v>
       </c>
-      <c r="Q28" s="12" t="s">
+      <c r="Q28" t="s">
         <v>204</v>
       </c>
     </row>
@@ -11358,7 +11354,7 @@
       <c r="O29" t="s">
         <v>281</v>
       </c>
-      <c r="P29" s="12" t="s">
+      <c r="P29" t="s">
         <v>58</v>
       </c>
     </row>
@@ -12290,7 +12286,7 @@
       <c r="O57" t="s">
         <v>425</v>
       </c>
-      <c r="P57" s="12" t="s">
+      <c r="P57" t="s">
         <v>58</v>
       </c>
     </row>
@@ -12331,7 +12327,7 @@
       <c r="O58" t="s">
         <v>434</v>
       </c>
-      <c r="Q58" s="12" t="s">
+      <c r="Q58" t="s">
         <v>435</v>
       </c>
     </row>
@@ -12527,7 +12523,7 @@
       <c r="O63" t="s">
         <v>468</v>
       </c>
-      <c r="Q63" s="12" t="s">
+      <c r="Q63" t="s">
         <v>469</v>
       </c>
     </row>
@@ -12559,7 +12555,7 @@
       <c r="O64" t="s">
         <v>473</v>
       </c>
-      <c r="Q64" s="12" t="s">
+      <c r="Q64" t="s">
         <v>469</v>
       </c>
     </row>
@@ -12591,7 +12587,7 @@
       <c r="O65" t="s">
         <v>477</v>
       </c>
-      <c r="Q65" s="12" t="s">
+      <c r="Q65" t="s">
         <v>469</v>
       </c>
     </row>
@@ -12679,7 +12675,7 @@
       <c r="O67" t="s">
         <v>496</v>
       </c>
-      <c r="P67" s="12" t="s">
+      <c r="P67" t="s">
         <v>497</v>
       </c>
     </row>
@@ -12723,7 +12719,7 @@
       <c r="O68" t="s">
         <v>504</v>
       </c>
-      <c r="P68" s="12" t="s">
+      <c r="P68" t="s">
         <v>497</v>
       </c>
     </row>
@@ -12767,7 +12763,7 @@
       <c r="O69" t="s">
         <v>510</v>
       </c>
-      <c r="P69" s="12" t="s">
+      <c r="P69" t="s">
         <v>497</v>
       </c>
     </row>
@@ -12811,7 +12807,7 @@
       <c r="O70" t="s">
         <v>520</v>
       </c>
-      <c r="Q70" s="12" t="s">
+      <c r="Q70" t="s">
         <v>521</v>
       </c>
     </row>
@@ -12855,7 +12851,7 @@
       <c r="O71" t="s">
         <v>528</v>
       </c>
-      <c r="P71" s="12" t="s">
+      <c r="P71" t="s">
         <v>497</v>
       </c>
     </row>
@@ -12899,10 +12895,10 @@
       <c r="O72" t="s">
         <v>539</v>
       </c>
-      <c r="P72" s="12" t="s">
+      <c r="P72" t="s">
         <v>540</v>
       </c>
-      <c r="Q72" s="12" t="s">
+      <c r="Q72" t="s">
         <v>541</v>
       </c>
     </row>
@@ -12940,7 +12936,7 @@
       <c r="O73" t="s">
         <v>550</v>
       </c>
-      <c r="Q73" s="12" t="s">
+      <c r="Q73" t="s">
         <v>139</v>
       </c>
     </row>
@@ -13227,10 +13223,10 @@
       <c r="O80" t="s">
         <v>610</v>
       </c>
-      <c r="P80" s="12" t="s">
+      <c r="P80" t="s">
         <v>611</v>
       </c>
-      <c r="Q80" s="12" t="s">
+      <c r="Q80" t="s">
         <v>612</v>
       </c>
     </row>
@@ -13309,7 +13305,7 @@
       <c r="O82" t="s">
         <v>630</v>
       </c>
-      <c r="Q82" s="12" t="s">
+      <c r="Q82" t="s">
         <v>139</v>
       </c>
     </row>
@@ -13347,7 +13343,7 @@
       <c r="O83" t="s">
         <v>639</v>
       </c>
-      <c r="Q83" s="12" t="s">
+      <c r="Q83" t="s">
         <v>640</v>
       </c>
     </row>
@@ -13385,7 +13381,7 @@
       <c r="O84" t="s">
         <v>646</v>
       </c>
-      <c r="Q84" s="12" t="s">
+      <c r="Q84" t="s">
         <v>647</v>
       </c>
     </row>
@@ -13589,7 +13585,7 @@
       <c r="O90" t="s">
         <v>700</v>
       </c>
-      <c r="Q90" s="12" t="s">
+      <c r="Q90" t="s">
         <v>139</v>
       </c>
     </row>
@@ -13674,7 +13670,7 @@
       <c r="O92" t="s">
         <v>718</v>
       </c>
-      <c r="P92" s="12" t="s">
+      <c r="P92" t="s">
         <v>58</v>
       </c>
     </row>
@@ -13808,10 +13804,10 @@
       <c r="O96" t="s">
         <v>744</v>
       </c>
-      <c r="P96" s="12" t="s">
+      <c r="P96" t="s">
         <v>745</v>
       </c>
-      <c r="Q96" s="12" t="s">
+      <c r="Q96" t="s">
         <v>746</v>
       </c>
     </row>
@@ -14062,7 +14058,7 @@
       <c r="O103" t="s">
         <v>800</v>
       </c>
-      <c r="Q103" s="12" t="s">
+      <c r="Q103" t="s">
         <v>801</v>
       </c>
     </row>
@@ -14147,7 +14143,7 @@
       <c r="O105" t="s">
         <v>819</v>
       </c>
-      <c r="P105" s="12" t="s">
+      <c r="P105" t="s">
         <v>820</v>
       </c>
     </row>
@@ -14191,7 +14187,7 @@
       <c r="O106" t="s">
         <v>827</v>
       </c>
-      <c r="P106" s="12" t="s">
+      <c r="P106" t="s">
         <v>828</v>
       </c>
     </row>
@@ -14459,7 +14455,7 @@
       <c r="O114" t="s">
         <v>884</v>
       </c>
-      <c r="P114" s="12" t="s">
+      <c r="P114" t="s">
         <v>820</v>
       </c>
     </row>
@@ -14602,7 +14598,7 @@
       <c r="O118" t="s">
         <v>909</v>
       </c>
-      <c r="Q118" s="12" t="s">
+      <c r="Q118" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14640,7 +14636,7 @@
       <c r="O119" t="s">
         <v>917</v>
       </c>
-      <c r="Q119" s="12" t="s">
+      <c r="Q119" t="s">
         <v>139</v>
       </c>
     </row>
@@ -14929,7 +14925,7 @@
       <c r="O127" t="s">
         <v>983</v>
       </c>
-      <c r="P127" s="12" t="s">
+      <c r="P127" t="s">
         <v>820</v>
       </c>
     </row>
@@ -14967,7 +14963,7 @@
       <c r="O128">
         <v>14</v>
       </c>
-      <c r="Q128" s="12" t="s">
+      <c r="Q128" t="s">
         <v>139</v>
       </c>
     </row>
@@ -15005,7 +15001,7 @@
       <c r="O129" t="s">
         <v>998</v>
       </c>
-      <c r="Q129" s="12" t="s">
+      <c r="Q129" t="s">
         <v>139</v>
       </c>
     </row>
@@ -15049,10 +15045,10 @@
       <c r="O130" t="s">
         <v>1006</v>
       </c>
-      <c r="P130" s="12" t="s">
+      <c r="P130" t="s">
         <v>1007</v>
       </c>
-      <c r="Q130" s="12" t="s">
+      <c r="Q130" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -15502,7 +15498,7 @@
       <c r="O142" t="s">
         <v>1093</v>
       </c>
-      <c r="P142" s="12" t="s">
+      <c r="P142" t="s">
         <v>820</v>
       </c>
     </row>
@@ -15675,7 +15671,7 @@
       <c r="O146" t="s">
         <v>1117</v>
       </c>
-      <c r="P146" s="12" t="s">
+      <c r="P146" t="s">
         <v>497</v>
       </c>
     </row>
@@ -15719,10 +15715,10 @@
       <c r="O147" t="s">
         <v>1124</v>
       </c>
-      <c r="P147" s="12" t="s">
+      <c r="P147" t="s">
         <v>1125</v>
       </c>
-      <c r="Q147" s="12" t="s">
+      <c r="Q147" t="s">
         <v>204</v>
       </c>
     </row>
@@ -15839,7 +15835,7 @@
       <c r="O150" t="s">
         <v>1149</v>
       </c>
-      <c r="P150" s="12" t="s">
+      <c r="P150" t="s">
         <v>820</v>
       </c>
     </row>
@@ -15915,7 +15911,7 @@
       <c r="O152" t="s">
         <v>1165</v>
       </c>
-      <c r="P152" s="12" t="s">
+      <c r="P152" t="s">
         <v>58</v>
       </c>
     </row>
@@ -16055,7 +16051,7 @@
       <c r="O156" t="s">
         <v>1190</v>
       </c>
-      <c r="Q156" s="12" t="s">
+      <c r="Q156" t="s">
         <v>1191</v>
       </c>
     </row>
@@ -16723,7 +16719,7 @@
       <c r="O175" t="s">
         <v>1312</v>
       </c>
-      <c r="Q175" s="12" t="s">
+      <c r="Q175" t="s">
         <v>139</v>
       </c>
     </row>
@@ -16799,7 +16795,7 @@
       <c r="O177" t="s">
         <v>1327</v>
       </c>
-      <c r="Q177" s="12" t="s">
+      <c r="Q177" t="s">
         <v>139</v>
       </c>
     </row>
@@ -17080,7 +17076,7 @@
       <c r="O184" t="s">
         <v>1381</v>
       </c>
-      <c r="Q184" s="12" t="s">
+      <c r="Q184" t="s">
         <v>139</v>
       </c>
     </row>
@@ -17124,10 +17120,10 @@
       <c r="O185" t="s">
         <v>1390</v>
       </c>
-      <c r="P185" s="12" t="s">
+      <c r="P185" t="s">
         <v>1391</v>
       </c>
-      <c r="Q185" s="12" t="s">
+      <c r="Q185" t="s">
         <v>1392</v>
       </c>
     </row>
@@ -17238,10 +17234,10 @@
       <c r="O188" t="s">
         <v>1411</v>
       </c>
-      <c r="P188" s="12" t="s">
+      <c r="P188" t="s">
         <v>1412</v>
       </c>
-      <c r="Q188" s="12" t="s">
+      <c r="Q188" t="s">
         <v>1413</v>
       </c>
     </row>
@@ -17355,7 +17351,7 @@
       <c r="O191" t="s">
         <v>1434</v>
       </c>
-      <c r="Q191" s="12" t="s">
+      <c r="Q191" t="s">
         <v>139</v>
       </c>
     </row>
@@ -17720,7 +17716,7 @@
       <c r="O201" t="s">
         <v>1513</v>
       </c>
-      <c r="Q201" s="12" t="s">
+      <c r="Q201" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -17758,7 +17754,7 @@
       <c r="O202" t="s">
         <v>1518</v>
       </c>
-      <c r="Q202" s="12" t="s">
+      <c r="Q202" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -17837,7 +17833,7 @@
       <c r="O204" t="s">
         <v>1535</v>
       </c>
-      <c r="P204" s="12" t="s">
+      <c r="P204" t="s">
         <v>58</v>
       </c>
     </row>
@@ -17881,7 +17877,7 @@
       <c r="O205" t="s">
         <v>1537</v>
       </c>
-      <c r="P205" s="12" t="s">
+      <c r="P205" t="s">
         <v>58</v>
       </c>
     </row>
@@ -17925,7 +17921,7 @@
       <c r="O206" t="s">
         <v>1543</v>
       </c>
-      <c r="P206" s="12" t="s">
+      <c r="P206" t="s">
         <v>58</v>
       </c>
     </row>
@@ -17969,7 +17965,7 @@
       <c r="O207" t="s">
         <v>1545</v>
       </c>
-      <c r="P207" s="12" t="s">
+      <c r="P207" t="s">
         <v>58</v>
       </c>
     </row>
@@ -18013,7 +18009,7 @@
       <c r="O208" t="s">
         <v>1547</v>
       </c>
-      <c r="P208" s="12" t="s">
+      <c r="P208" t="s">
         <v>58</v>
       </c>
     </row>
@@ -18086,7 +18082,7 @@
       <c r="O210" t="s">
         <v>1561</v>
       </c>
-      <c r="Q210" s="12" t="s">
+      <c r="Q210" t="s">
         <v>139</v>
       </c>
     </row>
@@ -18381,7 +18377,7 @@
       <c r="O218" t="s">
         <v>1603</v>
       </c>
-      <c r="Q218" s="12" t="s">
+      <c r="Q218" t="s">
         <v>1604</v>
       </c>
     </row>
@@ -18413,7 +18409,7 @@
       <c r="O219" t="s">
         <v>1612</v>
       </c>
-      <c r="Q219" s="12" t="s">
+      <c r="Q219" t="s">
         <v>1613</v>
       </c>
     </row>
@@ -18699,7 +18695,7 @@
       <c r="O227" t="s">
         <v>1513</v>
       </c>
-      <c r="Q227" s="12" t="s">
+      <c r="Q227" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -18743,7 +18739,7 @@
       <c r="O228" t="s">
         <v>1518</v>
       </c>
-      <c r="Q228" s="12" t="s">
+      <c r="Q228" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -18784,10 +18780,10 @@
       <c r="O229" t="s">
         <v>1670</v>
       </c>
-      <c r="P229" s="12" t="s">
+      <c r="P229" t="s">
         <v>1671</v>
       </c>
-      <c r="Q229" s="12" t="s">
+      <c r="Q229" t="s">
         <v>1672</v>
       </c>
       <c r="R229" t="s">
@@ -19025,7 +19021,7 @@
       <c r="N234" t="s">
         <v>1715</v>
       </c>
-      <c r="Q234" s="12" t="s">
+      <c r="Q234" t="s">
         <v>1716</v>
       </c>
     </row>
@@ -19063,10 +19059,10 @@
       <c r="N235" t="s">
         <v>1721</v>
       </c>
-      <c r="P235" s="12" t="s">
+      <c r="P235" t="s">
         <v>1722</v>
       </c>
-      <c r="Q235" s="12" t="s">
+      <c r="Q235" t="s">
         <v>1723</v>
       </c>
       <c r="AE235" t="s">
@@ -19404,7 +19400,7 @@
       <c r="O242" t="s">
         <v>1779</v>
       </c>
-      <c r="Q242" s="12" t="s">
+      <c r="Q242" t="s">
         <v>1780</v>
       </c>
       <c r="AE242" t="s">
@@ -19457,7 +19453,7 @@
       <c r="O243" t="s">
         <v>1789</v>
       </c>
-      <c r="Q243" s="12" t="s">
+      <c r="Q243" t="s">
         <v>1790</v>
       </c>
       <c r="AE243" t="s">
@@ -19510,7 +19506,7 @@
       <c r="O244" t="s">
         <v>1797</v>
       </c>
-      <c r="Q244" s="12" t="s">
+      <c r="Q244" t="s">
         <v>1798</v>
       </c>
       <c r="AE244" t="s">
@@ -19560,7 +19556,7 @@
       <c r="O245" t="s">
         <v>1805</v>
       </c>
-      <c r="Q245" s="12" t="s">
+      <c r="Q245" t="s">
         <v>1806</v>
       </c>
       <c r="AE245" t="s">
@@ -19977,7 +19973,7 @@
       <c r="O254" t="s">
         <v>1871</v>
       </c>
-      <c r="P254" s="12" t="s">
+      <c r="P254" t="s">
         <v>1872</v>
       </c>
     </row>
@@ -20018,7 +20014,7 @@
       <c r="O255" t="s">
         <v>1878</v>
       </c>
-      <c r="P255" s="12" t="s">
+      <c r="P255" t="s">
         <v>1879</v>
       </c>
       <c r="AE255" t="s">
@@ -20068,7 +20064,7 @@
       <c r="O256" t="s">
         <v>1888</v>
       </c>
-      <c r="P256" s="12" t="s">
+      <c r="P256" t="s">
         <v>1879</v>
       </c>
       <c r="AE256" t="s">
@@ -20435,10 +20431,10 @@
       <c r="N264" t="s">
         <v>717</v>
       </c>
-      <c r="P264" s="12" t="s">
+      <c r="P264" t="s">
         <v>58</v>
       </c>
-      <c r="Q264" s="12" t="s">
+      <c r="Q264" t="s">
         <v>1941</v>
       </c>
       <c r="AE264" t="s">
@@ -20532,7 +20528,7 @@
       <c r="O266" t="s">
         <v>1958</v>
       </c>
-      <c r="Q266" s="12" t="s">
+      <c r="Q266" t="s">
         <v>1959</v>
       </c>
       <c r="AE266" t="s">
@@ -20582,7 +20578,7 @@
       <c r="O267" t="s">
         <v>1967</v>
       </c>
-      <c r="Q267" s="12" t="s">
+      <c r="Q267" t="s">
         <v>1968</v>
       </c>
       <c r="AE267" t="s">
@@ -20679,7 +20675,7 @@
       <c r="O269">
         <v>170</v>
       </c>
-      <c r="Q269" s="12" t="s">
+      <c r="Q269" t="s">
         <v>1980</v>
       </c>
       <c r="AE269" t="s">
@@ -21563,7 +21559,7 @@
       <c r="O288" t="s">
         <v>2134</v>
       </c>
-      <c r="Q288" s="12" t="s">
+      <c r="Q288" t="s">
         <v>2135</v>
       </c>
       <c r="AE288" t="s">
@@ -21754,7 +21750,7 @@
       <c r="O292" t="s">
         <v>2143</v>
       </c>
-      <c r="Q292" s="12" t="s">
+      <c r="Q292" t="s">
         <v>2166</v>
       </c>
       <c r="R292" t="s">
@@ -21881,7 +21877,7 @@
       <c r="O294" t="s">
         <v>2188</v>
       </c>
-      <c r="Q294" s="12" t="s">
+      <c r="Q294" t="s">
         <v>2189</v>
       </c>
       <c r="AE294" t="s">
@@ -22260,7 +22256,7 @@
       <c r="O302" t="s">
         <v>2252</v>
       </c>
-      <c r="Q302" s="12" t="s">
+      <c r="Q302" t="s">
         <v>2253</v>
       </c>
       <c r="AE302" t="s">
@@ -23082,7 +23078,7 @@
       <c r="O320" t="s">
         <v>2363</v>
       </c>
-      <c r="Q320" s="12" t="s">
+      <c r="Q320" t="s">
         <v>2364</v>
       </c>
     </row>
@@ -23720,7 +23716,7 @@
       <c r="O333" t="s">
         <v>2456</v>
       </c>
-      <c r="Q333" s="12" t="s">
+      <c r="Q333" t="s">
         <v>2457</v>
       </c>
     </row>
@@ -23911,7 +23907,7 @@
       <c r="O337" t="s">
         <v>1741</v>
       </c>
-      <c r="Q337" s="12" t="s">
+      <c r="Q337" t="s">
         <v>2476</v>
       </c>
       <c r="AE337" t="s">
@@ -24630,7 +24626,7 @@
       <c r="O350" t="s">
         <v>2572</v>
       </c>
-      <c r="Q350" s="12" t="s">
+      <c r="Q350" t="s">
         <v>2573</v>
       </c>
       <c r="R350" t="s">
@@ -24852,7 +24848,7 @@
       <c r="O353" t="s">
         <v>2598</v>
       </c>
-      <c r="Q353" s="12" t="s">
+      <c r="Q353" t="s">
         <v>2599</v>
       </c>
       <c r="R353" t="s">
@@ -24932,7 +24928,7 @@
       <c r="O354" t="s">
         <v>2605</v>
       </c>
-      <c r="Q354" s="12" t="s">
+      <c r="Q354" t="s">
         <v>2606</v>
       </c>
       <c r="R354" t="s">
@@ -25006,7 +25002,7 @@
       <c r="O355" t="s">
         <v>2614</v>
       </c>
-      <c r="Q355" s="12" t="s">
+      <c r="Q355" t="s">
         <v>2615</v>
       </c>
       <c r="R355" t="s">
@@ -25512,7 +25508,7 @@
       <c r="O362" t="s">
         <v>2674</v>
       </c>
-      <c r="Q362" s="12" t="s">
+      <c r="Q362" t="s">
         <v>2675</v>
       </c>
       <c r="R362" t="s">
@@ -25867,7 +25863,7 @@
       <c r="N367" t="s">
         <v>2709</v>
       </c>
-      <c r="Q367" s="12" t="s">
+      <c r="Q367" t="s">
         <v>2710</v>
       </c>
       <c r="R367" t="s">
@@ -25941,7 +25937,7 @@
       <c r="O368" t="s">
         <v>2719</v>
       </c>
-      <c r="Q368" s="12" t="s">
+      <c r="Q368" t="s">
         <v>2720</v>
       </c>
       <c r="R368" t="s">
@@ -26737,7 +26733,7 @@
       <c r="O379" t="s">
         <v>2800</v>
       </c>
-      <c r="Q379" s="12" t="s">
+      <c r="Q379" t="s">
         <v>2801</v>
       </c>
       <c r="R379" t="s">
@@ -26817,7 +26813,7 @@
       <c r="O380" t="s">
         <v>2808</v>
       </c>
-      <c r="Q380" s="12" t="s">
+      <c r="Q380" t="s">
         <v>2801</v>
       </c>
       <c r="R380" t="s">
@@ -26959,7 +26955,7 @@
       <c r="O382" t="s">
         <v>2823</v>
       </c>
-      <c r="Q382" s="12" t="s">
+      <c r="Q382" t="s">
         <v>2824</v>
       </c>
       <c r="AE382" t="s">
@@ -27006,7 +27002,7 @@
       <c r="O383" t="s">
         <v>2832</v>
       </c>
-      <c r="Q383" s="12" t="s">
+      <c r="Q383" t="s">
         <v>2833</v>
       </c>
       <c r="AE383" t="s">
@@ -27097,10 +27093,10 @@
       <c r="O385" t="s">
         <v>2850</v>
       </c>
-      <c r="P385" s="12" t="s">
+      <c r="P385" t="s">
         <v>2851</v>
       </c>
-      <c r="Q385" s="12" t="s">
+      <c r="Q385" t="s">
         <v>2852</v>
       </c>
       <c r="AE385" t="s">
@@ -27238,7 +27234,7 @@
       <c r="O388" t="s">
         <v>2874</v>
       </c>
-      <c r="Q388" s="12" t="s">
+      <c r="Q388" t="s">
         <v>2875</v>
       </c>
       <c r="AE388" t="s">
@@ -27285,7 +27281,7 @@
       <c r="O389" t="s">
         <v>2883</v>
       </c>
-      <c r="Q389" s="12" t="s">
+      <c r="Q389" t="s">
         <v>2884</v>
       </c>
       <c r="AE389" t="s">
@@ -27332,7 +27328,7 @@
       <c r="O390" t="s">
         <v>2891</v>
       </c>
-      <c r="Q390" s="12" t="s">
+      <c r="Q390" t="s">
         <v>2892</v>
       </c>
       <c r="AE390" t="s">
@@ -27420,7 +27416,7 @@
       <c r="O392" t="s">
         <v>2906</v>
       </c>
-      <c r="Q392" s="12" t="s">
+      <c r="Q392" t="s">
         <v>2907</v>
       </c>
       <c r="AE392" t="s">
@@ -27471,8 +27467,8 @@
       <c r="O393" s="7" t="s">
         <v>2924</v>
       </c>
-      <c r="P393" s="13"/>
-      <c r="Q393" s="13"/>
+      <c r="P393" s="6"/>
+      <c r="Q393" s="6"/>
       <c r="R393" s="6"/>
       <c r="S393" s="6"/>
       <c r="T393" s="6"/>
@@ -27554,8 +27550,8 @@
       <c r="O394" s="6" t="s">
         <v>2400</v>
       </c>
-      <c r="P394" s="13"/>
-      <c r="Q394" s="13"/>
+      <c r="P394" s="6"/>
+      <c r="Q394" s="6"/>
       <c r="R394" s="6"/>
       <c r="S394" s="6"/>
       <c r="T394" s="6"/>
@@ -27629,8 +27625,8 @@
       <c r="O395" s="6" t="s">
         <v>2932</v>
       </c>
-      <c r="P395" s="13"/>
-      <c r="Q395" s="13"/>
+      <c r="P395" s="6"/>
+      <c r="Q395" s="6"/>
       <c r="R395" s="6"/>
       <c r="S395" s="6"/>
       <c r="T395" s="6"/>
@@ -27704,8 +27700,8 @@
       <c r="O396" s="6" t="s">
         <v>2937</v>
       </c>
-      <c r="P396" s="13"/>
-      <c r="Q396" s="13" t="s">
+      <c r="P396" s="6"/>
+      <c r="Q396" s="6" t="s">
         <v>2967</v>
       </c>
       <c r="R396" s="6"/>
@@ -27781,8 +27777,8 @@
       <c r="O397" s="6" t="s">
         <v>2945</v>
       </c>
-      <c r="P397" s="13"/>
-      <c r="Q397" s="13"/>
+      <c r="P397" s="6"/>
+      <c r="Q397" s="6"/>
       <c r="R397" s="6"/>
       <c r="S397" s="6"/>
       <c r="T397" s="6"/>
@@ -27856,8 +27852,8 @@
       <c r="O398" s="6" t="s">
         <v>2947</v>
       </c>
-      <c r="P398" s="13"/>
-      <c r="Q398" s="13" t="s">
+      <c r="P398" s="6"/>
+      <c r="Q398" s="6" t="s">
         <v>2948</v>
       </c>
       <c r="R398" s="6"/>
@@ -27933,8 +27929,8 @@
       <c r="O399" s="6" t="s">
         <v>2957</v>
       </c>
-      <c r="P399" s="13"/>
-      <c r="Q399" s="13" t="s">
+      <c r="P399" s="6"/>
+      <c r="Q399" s="6" t="s">
         <v>2955</v>
       </c>
       <c r="R399" s="6"/>
@@ -28010,8 +28006,8 @@
       <c r="O400" s="6" t="s">
         <v>2962</v>
       </c>
-      <c r="P400" s="13"/>
-      <c r="Q400" s="13" t="s">
+      <c r="P400" s="6"/>
+      <c r="Q400" s="6" t="s">
         <v>2963</v>
       </c>
       <c r="R400" s="6"/>
@@ -28087,8 +28083,8 @@
       <c r="O401" s="6" t="s">
         <v>2972</v>
       </c>
-      <c r="P401" s="13"/>
-      <c r="Q401" s="13"/>
+      <c r="P401" s="6"/>
+      <c r="Q401" s="6"/>
       <c r="R401" s="6"/>
       <c r="S401" s="6"/>
       <c r="T401" s="6"/>
@@ -28162,8 +28158,8 @@
       <c r="O402" s="6" t="s">
         <v>2974</v>
       </c>
-      <c r="P402" s="13"/>
-      <c r="Q402" s="13"/>
+      <c r="P402" s="6"/>
+      <c r="Q402" s="6"/>
       <c r="R402" s="6"/>
       <c r="S402" s="6"/>
       <c r="T402" s="6"/>
@@ -28237,8 +28233,8 @@
       <c r="O403" s="6" t="s">
         <v>2980</v>
       </c>
-      <c r="P403" s="13"/>
-      <c r="Q403" s="13"/>
+      <c r="P403" s="6"/>
+      <c r="Q403" s="6"/>
       <c r="R403" s="6"/>
       <c r="S403" s="6"/>
       <c r="T403" s="6"/>
@@ -28316,8 +28312,8 @@
       <c r="O404" s="6" t="s">
         <v>2988</v>
       </c>
-      <c r="P404" s="13"/>
-      <c r="Q404" s="13"/>
+      <c r="P404" s="6"/>
+      <c r="Q404" s="6"/>
       <c r="R404" s="6"/>
       <c r="S404" s="6"/>
       <c r="T404" s="6"/>
@@ -28391,8 +28387,8 @@
       <c r="O405" s="6" t="s">
         <v>2998</v>
       </c>
-      <c r="P405" s="13"/>
-      <c r="Q405" s="13" t="s">
+      <c r="P405" s="6"/>
+      <c r="Q405" s="6" t="s">
         <v>2999</v>
       </c>
       <c r="R405" s="6"/>
@@ -28466,8 +28462,8 @@
       <c r="O406" s="6" t="s">
         <v>3012</v>
       </c>
-      <c r="P406" s="13"/>
-      <c r="Q406" s="13" t="s">
+      <c r="P406" s="6"/>
+      <c r="Q406" s="6" t="s">
         <v>3005</v>
       </c>
       <c r="R406" s="6"/>
@@ -28543,8 +28539,8 @@
       <c r="O407" s="6" t="s">
         <v>3015</v>
       </c>
-      <c r="P407" s="13"/>
-      <c r="Q407" s="13" t="s">
+      <c r="P407" s="6"/>
+      <c r="Q407" s="6" t="s">
         <v>3021</v>
       </c>
       <c r="R407" s="6"/>
@@ -28620,10 +28616,10 @@
       <c r="O408" s="6" t="s">
         <v>3028</v>
       </c>
-      <c r="P408" s="13" t="s">
+      <c r="P408" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q408" s="14" t="s">
+      <c r="Q408" s="11" t="s">
         <v>3002</v>
       </c>
       <c r="R408" s="6"/>
@@ -28699,8 +28695,8 @@
       <c r="O409" s="6" t="s">
         <v>3031</v>
       </c>
-      <c r="P409" s="13"/>
-      <c r="Q409" s="13"/>
+      <c r="P409" s="6"/>
+      <c r="Q409" s="6"/>
       <c r="R409" s="6"/>
       <c r="S409" s="6"/>
       <c r="T409" s="6"/>
@@ -28774,10 +28770,10 @@
       <c r="O410" s="6" t="s">
         <v>3039</v>
       </c>
-      <c r="P410" s="13" t="s">
+      <c r="P410" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q410" s="13"/>
+      <c r="Q410" s="6"/>
       <c r="R410" s="6"/>
       <c r="S410" s="6"/>
       <c r="T410" s="6"/>
@@ -28851,10 +28847,10 @@
       <c r="O411" s="6" t="s">
         <v>3048</v>
       </c>
-      <c r="P411" s="13" t="s">
+      <c r="P411" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q411" s="13" t="s">
+      <c r="Q411" s="6" t="s">
         <v>3075</v>
       </c>
       <c r="R411" s="6"/>
@@ -28930,10 +28926,10 @@
       <c r="O412" s="6" t="s">
         <v>3049</v>
       </c>
-      <c r="P412" s="13" t="s">
+      <c r="P412" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q412" s="13" t="s">
+      <c r="Q412" s="6" t="s">
         <v>3074</v>
       </c>
       <c r="R412" s="6"/>
@@ -29009,10 +29005,10 @@
       <c r="O413" s="6" t="s">
         <v>3054</v>
       </c>
-      <c r="P413" s="13" t="s">
+      <c r="P413" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q413" s="13" t="s">
+      <c r="Q413" s="6" t="s">
         <v>3000</v>
       </c>
       <c r="R413" s="6"/>
@@ -29088,10 +29084,10 @@
       <c r="O414" s="6" t="s">
         <v>3059</v>
       </c>
-      <c r="P414" s="13" t="s">
+      <c r="P414" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q414" s="13" t="s">
+      <c r="Q414" s="6" t="s">
         <v>3076</v>
       </c>
       <c r="R414" s="6"/>
@@ -29167,10 +29163,10 @@
       <c r="O415" s="6" t="s">
         <v>3064</v>
       </c>
-      <c r="P415" s="13" t="s">
+      <c r="P415" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q415" s="13" t="s">
+      <c r="Q415" s="6" t="s">
         <v>3001</v>
       </c>
       <c r="R415" s="6"/>
@@ -29246,10 +29242,10 @@
       <c r="O416" s="6" t="s">
         <v>3072</v>
       </c>
-      <c r="P416" s="13" t="s">
+      <c r="P416" s="6" t="s">
         <v>3073</v>
       </c>
-      <c r="Q416" s="13" t="s">
+      <c r="Q416" s="6" t="s">
         <v>3077</v>
       </c>
       <c r="R416" s="6"/>
@@ -29303,8 +29299,8 @@
       <c r="M417" s="6"/>
       <c r="N417" s="6"/>
       <c r="O417" s="6"/>
-      <c r="P417" s="13"/>
-      <c r="Q417" s="13"/>
+      <c r="P417" s="6"/>
+      <c r="Q417" s="6"/>
       <c r="R417" s="6"/>
       <c r="S417" s="6"/>
       <c r="T417" s="6"/>
@@ -29356,8 +29352,8 @@
       <c r="M418" s="6"/>
       <c r="N418" s="6"/>
       <c r="O418" s="6"/>
-      <c r="P418" s="13"/>
-      <c r="Q418" s="13"/>
+      <c r="P418" s="6"/>
+      <c r="Q418" s="6"/>
       <c r="R418" s="6"/>
       <c r="S418" s="6"/>
       <c r="T418" s="6"/>
@@ -29409,8 +29405,8 @@
       <c r="M419" s="6"/>
       <c r="N419" s="6"/>
       <c r="O419" s="6"/>
-      <c r="P419" s="13"/>
-      <c r="Q419" s="13"/>
+      <c r="P419" s="6"/>
+      <c r="Q419" s="6"/>
       <c r="R419" s="6"/>
       <c r="S419" s="6"/>
       <c r="T419" s="6"/>
@@ -29462,8 +29458,8 @@
       <c r="M420" s="6"/>
       <c r="N420" s="6"/>
       <c r="O420" s="6"/>
-      <c r="P420" s="13"/>
-      <c r="Q420" s="13"/>
+      <c r="P420" s="6"/>
+      <c r="Q420" s="6"/>
       <c r="R420" s="6"/>
       <c r="S420" s="6"/>
       <c r="T420" s="6"/>
@@ -29515,8 +29511,8 @@
       <c r="M421" s="6"/>
       <c r="N421" s="6"/>
       <c r="O421" s="6"/>
-      <c r="P421" s="13"/>
-      <c r="Q421" s="13"/>
+      <c r="P421" s="6"/>
+      <c r="Q421" s="6"/>
       <c r="R421" s="6"/>
       <c r="S421" s="6"/>
       <c r="T421" s="6"/>
@@ -29568,8 +29564,8 @@
       <c r="M422" s="6"/>
       <c r="N422" s="6"/>
       <c r="O422" s="6"/>
-      <c r="P422" s="13"/>
-      <c r="Q422" s="13"/>
+      <c r="P422" s="6"/>
+      <c r="Q422" s="6"/>
       <c r="R422" s="6"/>
       <c r="S422" s="6"/>
       <c r="T422" s="6"/>
@@ -29621,8 +29617,8 @@
       <c r="M423" s="6"/>
       <c r="N423" s="6"/>
       <c r="O423" s="6"/>
-      <c r="P423" s="13"/>
-      <c r="Q423" s="13"/>
+      <c r="P423" s="6"/>
+      <c r="Q423" s="6"/>
       <c r="R423" s="6"/>
       <c r="S423" s="6"/>
       <c r="T423" s="6"/>
@@ -29674,8 +29670,8 @@
       <c r="M424" s="6"/>
       <c r="N424" s="6"/>
       <c r="O424" s="6"/>
-      <c r="P424" s="13"/>
-      <c r="Q424" s="13"/>
+      <c r="P424" s="6"/>
+      <c r="Q424" s="6"/>
       <c r="R424" s="6"/>
       <c r="S424" s="6"/>
       <c r="T424" s="6"/>
@@ -29727,8 +29723,8 @@
       <c r="M425" s="6"/>
       <c r="N425" s="6"/>
       <c r="O425" s="6"/>
-      <c r="P425" s="13"/>
-      <c r="Q425" s="13"/>
+      <c r="P425" s="6"/>
+      <c r="Q425" s="6"/>
       <c r="R425" s="6"/>
       <c r="S425" s="6"/>
       <c r="T425" s="6"/>
@@ -29780,8 +29776,8 @@
       <c r="M426" s="6"/>
       <c r="N426" s="6"/>
       <c r="O426" s="6"/>
-      <c r="P426" s="13"/>
-      <c r="Q426" s="13"/>
+      <c r="P426" s="6"/>
+      <c r="Q426" s="6"/>
       <c r="R426" s="6"/>
       <c r="S426" s="6"/>
       <c r="T426" s="6"/>
@@ -29833,8 +29829,8 @@
       <c r="M427" s="6"/>
       <c r="N427" s="6"/>
       <c r="O427" s="6"/>
-      <c r="P427" s="13"/>
-      <c r="Q427" s="13"/>
+      <c r="P427" s="6"/>
+      <c r="Q427" s="6"/>
       <c r="R427" s="6"/>
       <c r="S427" s="6"/>
       <c r="T427" s="6"/>

</xml_diff>

<commit_message>
updated power source table
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/species_list_10071623_NJMg.xlsx
+++ b/flag/AQB_classification/species_list_10071623_NJMg.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/bioinfRhints/flag/AQB_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D22A9D-6E9C-5047-8925-6D65D7D4D811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403ED804-39CF-DA42-A66C-E412DA170AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="5320" windowWidth="35160" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6200" yWindow="500" windowWidth="35160" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_list_10071623_NJMf" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5663" uniqueCount="3078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5676" uniqueCount="3082">
   <si>
     <t>Download script?</t>
   </si>
@@ -8973,10 +8986,6 @@
   </si>
   <si>
     <t>Ito, Takahashi 2017</t>
-  </si>
-  <si>
-    <t>Mg2+_or_Ca2+_or_Sr2+ (MotA1, GAK41226.1);
-H+ (MotA2, GAK43333.1)</t>
   </si>
   <si>
     <t>powerSource; Ito &amp; Takahashi 2017, Fig. 4</t>
@@ -9259,6 +9268,22 @@
   </si>
   <si>
     <t>formerly Sphingobium barthaii KK22; "Sphingobium fuliginis produces an organophosphate hydrolase (OPH) to degrade organophosphate insecticides and nerve agents. OPH is targeted to the CM of E. coli when it is coexpressed with either ExbD or ExbB ExbD (65). "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerSource "Mg2+_or_Ca2+_or_Sr2+ (MotA1, GAK41226.1);
+H+ (MotA2, GAK43333.1)" </t>
+  </si>
+  <si>
+    <t>bication</t>
+  </si>
+  <si>
+    <t>Contains very close match to ACJ39421.1 PomA2 [Aeromonas piscicola-traced to Aeromonas hydrophila strain AH-3, but genome fails checks], of reference</t>
+  </si>
+  <si>
+    <t>Wilhelms M, Vilches S, Molero R, et al. Two redundant sodium-driven stator motor proteins are involved in Aeromonas hydrophila polar flagellum rotation. Journal of Bacteriology. 2009 Apr;191(7):2206-2217 https://europepmc.org/article/PMC/2655530#data</t>
+  </si>
+  <si>
+    <t>2023-08-05_NJM</t>
   </si>
 </sst>
 </file>
@@ -10163,10 +10188,10 @@
   <dimension ref="A1:AY439"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="15" ySplit="1" topLeftCell="Z378" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="15" ySplit="1" topLeftCell="P416" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K391" sqref="K391"/>
+      <selection pane="bottomRight" activeCell="K426" sqref="K426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19360,7 +19385,7 @@
         <v>1774</v>
       </c>
       <c r="AH241" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="242" spans="2:34" x14ac:dyDescent="0.2">
@@ -22125,7 +22150,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="300" spans="2:34" ht="136" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:34" ht="170" x14ac:dyDescent="0.2">
       <c r="B300" t="s">
         <v>1942</v>
       </c>
@@ -22166,10 +22191,10 @@
         <v>2236</v>
       </c>
       <c r="AG300" s="3" t="s">
-        <v>2984</v>
-      </c>
-      <c r="AH300" t="s">
-        <v>1686</v>
+        <v>3078</v>
+      </c>
+      <c r="AH300" s="3" t="s">
+        <v>3077</v>
       </c>
     </row>
     <row r="301" spans="2:34" x14ac:dyDescent="0.2">
@@ -23126,7 +23151,7 @@
         <v>2371</v>
       </c>
       <c r="AG321" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="AH321" t="s">
         <v>1686</v>
@@ -28280,14 +28305,14 @@
         <v>2930</v>
       </c>
       <c r="C404" s="6" t="s">
+        <v>2990</v>
+      </c>
+      <c r="D404" s="6" t="s">
         <v>2991</v>
-      </c>
-      <c r="D404" s="6" t="s">
-        <v>2992</v>
       </c>
       <c r="E404" s="6"/>
       <c r="F404" s="6" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="G404" s="6"/>
       <c r="H404" s="6"/>
@@ -28298,19 +28323,19 @@
         <v>258</v>
       </c>
       <c r="K404" s="6" t="s">
+        <v>2988</v>
+      </c>
+      <c r="L404" s="6" t="s">
         <v>2989</v>
       </c>
-      <c r="L404" s="6" t="s">
-        <v>2990</v>
-      </c>
       <c r="M404" s="6" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="N404" s="6" t="s">
         <v>732</v>
       </c>
       <c r="O404" s="6" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="P404" s="6"/>
       <c r="Q404" s="6"/>
@@ -28355,14 +28380,14 @@
         <v>2930</v>
       </c>
       <c r="C405" s="6" t="s">
+        <v>2993</v>
+      </c>
+      <c r="D405" s="6" t="s">
         <v>2994</v>
-      </c>
-      <c r="D405" s="6" t="s">
-        <v>2995</v>
       </c>
       <c r="E405" s="6"/>
       <c r="F405" s="6" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="G405" s="6"/>
       <c r="H405" s="6"/>
@@ -28382,14 +28407,14 @@
         <v>1769</v>
       </c>
       <c r="N405" s="6" t="s">
+        <v>2996</v>
+      </c>
+      <c r="O405" s="6" t="s">
         <v>2997</v>
-      </c>
-      <c r="O405" s="6" t="s">
-        <v>2998</v>
       </c>
       <c r="P405" s="6"/>
       <c r="Q405" s="6" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="R405" s="6"/>
       <c r="S405" s="6"/>
@@ -28432,39 +28457,39 @@
         <v>2930</v>
       </c>
       <c r="C406" s="6" t="s">
+        <v>3006</v>
+      </c>
+      <c r="D406" s="6" t="s">
         <v>3007</v>
-      </c>
-      <c r="D406" s="6" t="s">
-        <v>3008</v>
       </c>
       <c r="E406" s="6"/>
       <c r="F406" s="6" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="G406" s="6"/>
       <c r="H406" s="6"/>
       <c r="I406" s="8" t="s">
+        <v>3008</v>
+      </c>
+      <c r="J406" s="6" t="s">
         <v>3009</v>
       </c>
-      <c r="J406" s="6" t="s">
+      <c r="K406" s="6" t="s">
         <v>3010</v>
-      </c>
-      <c r="K406" s="6" t="s">
-        <v>3011</v>
       </c>
       <c r="L406" s="6"/>
       <c r="M406" s="6" t="s">
+        <v>3002</v>
+      </c>
+      <c r="N406" s="6" t="s">
         <v>3003</v>
       </c>
-      <c r="N406" s="6" t="s">
-        <v>3004</v>
-      </c>
       <c r="O406" s="6" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="P406" s="6"/>
       <c r="Q406" s="6" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="R406" s="6"/>
       <c r="S406" s="6"/>
@@ -28507,14 +28532,14 @@
         <v>2930</v>
       </c>
       <c r="C407" s="6" t="s">
+        <v>3017</v>
+      </c>
+      <c r="D407" s="6" t="s">
         <v>3018</v>
-      </c>
-      <c r="D407" s="6" t="s">
-        <v>3019</v>
       </c>
       <c r="E407" s="6"/>
       <c r="F407" s="6" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
       <c r="G407" s="6"/>
       <c r="H407" s="6"/>
@@ -28525,23 +28550,23 @@
         <v>85</v>
       </c>
       <c r="K407" s="6" t="s">
+        <v>3015</v>
+      </c>
+      <c r="L407" s="6" t="s">
         <v>3016</v>
       </c>
-      <c r="L407" s="6" t="s">
-        <v>3017</v>
-      </c>
       <c r="M407" s="6" t="s">
+        <v>3012</v>
+      </c>
+      <c r="N407" s="6" t="s">
         <v>3013</v>
       </c>
-      <c r="N407" s="6" t="s">
+      <c r="O407" s="6" t="s">
         <v>3014</v>
-      </c>
-      <c r="O407" s="6" t="s">
-        <v>3015</v>
       </c>
       <c r="P407" s="6"/>
       <c r="Q407" s="6" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="R407" s="6"/>
       <c r="S407" s="6"/>
@@ -28584,14 +28609,14 @@
         <v>2930</v>
       </c>
       <c r="C408" s="6" t="s">
+        <v>3022</v>
+      </c>
+      <c r="D408" s="6" t="s">
         <v>3023</v>
-      </c>
-      <c r="D408" s="6" t="s">
-        <v>3024</v>
       </c>
       <c r="E408" s="6"/>
       <c r="F408" s="6" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
       <c r="G408" s="6"/>
       <c r="H408" s="6"/>
@@ -28599,28 +28624,28 @@
         <v>813</v>
       </c>
       <c r="J408" s="6" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="K408" s="6" t="s">
         <v>880</v>
       </c>
       <c r="L408" s="6" t="s">
+        <v>3025</v>
+      </c>
+      <c r="M408" s="6" t="s">
         <v>3026</v>
-      </c>
-      <c r="M408" s="6" t="s">
-        <v>3027</v>
       </c>
       <c r="N408" s="6" t="s">
         <v>1512</v>
       </c>
       <c r="O408" s="6" t="s">
-        <v>3028</v>
+        <v>3027</v>
       </c>
       <c r="P408" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q408" s="11" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="R408" s="6"/>
       <c r="S408" s="6"/>
@@ -28663,14 +28688,14 @@
         <v>2930</v>
       </c>
       <c r="C409" s="6" t="s">
+        <v>3031</v>
+      </c>
+      <c r="D409" s="6" t="s">
         <v>3032</v>
-      </c>
-      <c r="D409" s="6" t="s">
-        <v>3033</v>
       </c>
       <c r="E409" s="6"/>
       <c r="F409" s="6" t="s">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="G409" s="6"/>
       <c r="H409" s="6"/>
@@ -28678,22 +28703,22 @@
         <v>813</v>
       </c>
       <c r="J409" s="6" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="K409" s="6" t="s">
+        <v>3034</v>
+      </c>
+      <c r="L409" s="6" t="s">
         <v>3035</v>
       </c>
-      <c r="L409" s="6" t="s">
-        <v>3036</v>
-      </c>
       <c r="M409" s="6" t="s">
+        <v>3028</v>
+      </c>
+      <c r="N409" s="6" t="s">
         <v>3029</v>
       </c>
-      <c r="N409" s="6" t="s">
+      <c r="O409" s="6" t="s">
         <v>3030</v>
-      </c>
-      <c r="O409" s="6" t="s">
-        <v>3031</v>
       </c>
       <c r="P409" s="6"/>
       <c r="Q409" s="6"/>
@@ -28738,14 +28763,14 @@
         <v>2930</v>
       </c>
       <c r="C410" s="6" t="s">
+        <v>3040</v>
+      </c>
+      <c r="D410" s="6" t="s">
         <v>3041</v>
-      </c>
-      <c r="D410" s="6" t="s">
-        <v>3042</v>
       </c>
       <c r="E410" s="6"/>
       <c r="F410" s="6" t="s">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="G410" s="6"/>
       <c r="H410" s="6"/>
@@ -28753,25 +28778,25 @@
         <v>813</v>
       </c>
       <c r="J410" s="6" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="K410" s="6" t="s">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="L410" s="6" t="s">
-        <v>3040</v>
+        <v>3039</v>
       </c>
       <c r="M410" s="6" t="s">
-        <v>3038</v>
+        <v>3037</v>
       </c>
       <c r="N410" s="6" t="s">
         <v>1512</v>
       </c>
       <c r="O410" s="6" t="s">
-        <v>3039</v>
+        <v>3038</v>
       </c>
       <c r="P410" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q410" s="6"/>
       <c r="R410" s="6"/>
@@ -28815,14 +28840,14 @@
         <v>2930</v>
       </c>
       <c r="C411" s="6" t="s">
+        <v>3042</v>
+      </c>
+      <c r="D411" s="6" t="s">
         <v>3043</v>
-      </c>
-      <c r="D411" s="6" t="s">
-        <v>3044</v>
       </c>
       <c r="E411" s="6"/>
       <c r="F411" s="6" t="s">
-        <v>3045</v>
+        <v>3044</v>
       </c>
       <c r="G411" s="6"/>
       <c r="H411" s="6"/>
@@ -28836,22 +28861,22 @@
         <v>2148</v>
       </c>
       <c r="L411" s="6" t="s">
+        <v>3045</v>
+      </c>
+      <c r="M411" s="6" t="s">
         <v>3046</v>
-      </c>
-      <c r="M411" s="6" t="s">
-        <v>3047</v>
       </c>
       <c r="N411" s="6" t="s">
         <v>1181</v>
       </c>
       <c r="O411" s="6" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="P411" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q411" s="6" t="s">
-        <v>3075</v>
+        <v>3074</v>
       </c>
       <c r="R411" s="6"/>
       <c r="S411" s="6"/>
@@ -28894,14 +28919,14 @@
         <v>2930</v>
       </c>
       <c r="C412" s="6" t="s">
+        <v>3049</v>
+      </c>
+      <c r="D412" s="6" t="s">
         <v>3050</v>
-      </c>
-      <c r="D412" s="6" t="s">
-        <v>3051</v>
       </c>
       <c r="E412" s="6"/>
       <c r="F412" s="6" t="s">
-        <v>3052</v>
+        <v>3051</v>
       </c>
       <c r="G412" s="6"/>
       <c r="H412" s="6"/>
@@ -28924,13 +28949,13 @@
         <v>2353</v>
       </c>
       <c r="O412" s="6" t="s">
-        <v>3049</v>
+        <v>3048</v>
       </c>
       <c r="P412" s="6" t="s">
+        <v>3072</v>
+      </c>
+      <c r="Q412" s="6" t="s">
         <v>3073</v>
-      </c>
-      <c r="Q412" s="6" t="s">
-        <v>3074</v>
       </c>
       <c r="R412" s="6"/>
       <c r="S412" s="6"/>
@@ -28973,14 +28998,14 @@
         <v>2930</v>
       </c>
       <c r="C413" s="6" t="s">
+        <v>3055</v>
+      </c>
+      <c r="D413" s="6" t="s">
         <v>3056</v>
-      </c>
-      <c r="D413" s="6" t="s">
-        <v>3057</v>
       </c>
       <c r="E413" s="6"/>
       <c r="F413" s="6" t="s">
-        <v>3055</v>
+        <v>3054</v>
       </c>
       <c r="G413" s="6"/>
       <c r="H413" s="6"/>
@@ -28997,19 +29022,19 @@
         <v>1301</v>
       </c>
       <c r="M413" s="6" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="N413" s="6" t="s">
         <v>1512</v>
       </c>
       <c r="O413" s="6" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
       <c r="P413" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q413" s="6" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="R413" s="6"/>
       <c r="S413" s="6"/>
@@ -29052,14 +29077,14 @@
         <v>2930</v>
       </c>
       <c r="C414" s="6" t="s">
+        <v>3059</v>
+      </c>
+      <c r="D414" s="6" t="s">
         <v>3060</v>
-      </c>
-      <c r="D414" s="6" t="s">
-        <v>3061</v>
       </c>
       <c r="E414" s="6"/>
       <c r="F414" s="6" t="s">
-        <v>3062</v>
+        <v>3061</v>
       </c>
       <c r="G414" s="6"/>
       <c r="H414" s="6"/>
@@ -29079,16 +29104,16 @@
         <v>148</v>
       </c>
       <c r="N414" s="6" t="s">
+        <v>3057</v>
+      </c>
+      <c r="O414" s="6" t="s">
         <v>3058</v>
       </c>
-      <c r="O414" s="6" t="s">
-        <v>3059</v>
-      </c>
       <c r="P414" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q414" s="6" t="s">
-        <v>3076</v>
+        <v>3075</v>
       </c>
       <c r="R414" s="6"/>
       <c r="S414" s="6"/>
@@ -29131,14 +29156,14 @@
         <v>2930</v>
       </c>
       <c r="C415" s="6" t="s">
+        <v>3064</v>
+      </c>
+      <c r="D415" s="6" t="s">
         <v>3065</v>
-      </c>
-      <c r="D415" s="6" t="s">
-        <v>3066</v>
       </c>
       <c r="E415" s="6"/>
       <c r="F415" s="6" t="s">
-        <v>3067</v>
+        <v>3066</v>
       </c>
       <c r="G415" s="6"/>
       <c r="H415" s="6"/>
@@ -29158,16 +29183,16 @@
         <v>148</v>
       </c>
       <c r="N415" s="6" t="s">
+        <v>3062</v>
+      </c>
+      <c r="O415" s="6" t="s">
         <v>3063</v>
       </c>
-      <c r="O415" s="6" t="s">
-        <v>3064</v>
-      </c>
       <c r="P415" s="6" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="Q415" s="6" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="R415" s="6"/>
       <c r="S415" s="6"/>
@@ -29210,14 +29235,14 @@
         <v>2930</v>
       </c>
       <c r="C416" s="6" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D416" s="6" t="s">
-        <v>3068</v>
+        <v>3067</v>
       </c>
       <c r="E416" s="6"/>
       <c r="F416" s="6" t="s">
-        <v>3070</v>
+        <v>3069</v>
       </c>
       <c r="G416" s="6"/>
       <c r="H416" s="6"/>
@@ -29234,19 +29259,19 @@
         <v>1301</v>
       </c>
       <c r="M416" s="6" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="N416" s="6" t="s">
+        <v>3070</v>
+      </c>
+      <c r="O416" s="6" t="s">
         <v>3071</v>
       </c>
-      <c r="O416" s="6" t="s">
+      <c r="P416" s="6" t="s">
         <v>3072</v>
       </c>
-      <c r="P416" s="6" t="s">
-        <v>3073</v>
-      </c>
       <c r="Q416" s="6" t="s">
-        <v>3077</v>
+        <v>3076</v>
       </c>
       <c r="R416" s="6"/>
       <c r="S416" s="6"/>
@@ -29285,22 +29310,48 @@
     </row>
     <row r="417" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A417" s="6"/>
-      <c r="B417" s="6"/>
-      <c r="C417" s="6"/>
-      <c r="D417" s="6"/>
+      <c r="B417" s="6" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C417" s="6" t="s">
+        <v>2933</v>
+      </c>
+      <c r="D417" s="6" t="s">
+        <v>2934</v>
+      </c>
       <c r="E417" s="6"/>
-      <c r="F417" s="6"/>
+      <c r="F417" s="6" t="s">
+        <v>2935</v>
+      </c>
       <c r="G417" s="6"/>
       <c r="H417" s="6"/>
-      <c r="I417" s="8"/>
-      <c r="J417" s="6"/>
-      <c r="K417" s="6"/>
-      <c r="L417" s="6"/>
-      <c r="M417" s="6"/>
-      <c r="N417" s="6"/>
-      <c r="O417" s="6"/>
-      <c r="P417" s="6"/>
-      <c r="Q417" s="6"/>
+      <c r="I417" t="s">
+        <v>51</v>
+      </c>
+      <c r="J417" t="s">
+        <v>52</v>
+      </c>
+      <c r="K417" t="s">
+        <v>238</v>
+      </c>
+      <c r="L417" t="s">
+        <v>1680</v>
+      </c>
+      <c r="M417" t="s">
+        <v>1681</v>
+      </c>
+      <c r="N417" s="6" t="s">
+        <v>2936</v>
+      </c>
+      <c r="O417" s="6" t="s">
+        <v>2937</v>
+      </c>
+      <c r="P417" s="6" t="s">
+        <v>3080</v>
+      </c>
+      <c r="Q417" s="6" t="s">
+        <v>3079</v>
+      </c>
       <c r="R417" s="6"/>
       <c r="S417" s="6"/>
       <c r="T417" s="6"/>

</xml_diff>